<commit_message>
First push of release candidate: v2.0.0rc
</commit_message>
<xml_diff>
--- a/product-definitions/spreadsheet/aerosol-backscatter.xlsx
+++ b/product-definitions/spreadsheet/aerosol-backscatter.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="dimensions-specific" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="variables-specific" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="global-attributes-specific" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="dimensions-specific" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="variables-specific" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,29 +13,110 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Fixed Value</t>
+  </si>
+  <si>
+    <t>Compliance checking rules</t>
+  </si>
+  <si>
+    <t>Convention Providence</t>
+  </si>
+  <si>
+    <t>laser_wavelength</t>
+  </si>
+  <si>
+    <t>wavelength of ceilometer laser</t>
+  </si>
+  <si>
+    <t>910 nm</t>
+  </si>
+  <si>
+    <t>String: min 3 characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal_laser_pulse_energy </t>
+  </si>
+  <si>
+    <t>nominal laser pulse energy</t>
+  </si>
+  <si>
+    <t>3.0e-06 J</t>
+  </si>
+  <si>
+    <t>pulse_repetition_frequency</t>
+  </si>
+  <si>
+    <t>pulse repetition frequency</t>
+  </si>
+  <si>
+    <t>6500 s-1</t>
+  </si>
+  <si>
+    <t>lens_diameter</t>
+  </si>
+  <si>
+    <t>lens diameter</t>
+  </si>
+  <si>
+    <t>0.148 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beam_divergence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">beam divergence </t>
+  </si>
+  <si>
+    <t>0.14 degrees</t>
+  </si>
+  <si>
+    <t>pulse_length</t>
+  </si>
+  <si>
+    <t>pulse length</t>
+  </si>
+  <si>
+    <t>1.1e-07 s</t>
+  </si>
+  <si>
+    <t>sampling_frequency</t>
+  </si>
+  <si>
+    <t>sampling frequency</t>
+  </si>
+  <si>
+    <t>1.5e+07 s-1</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>altitude</t>
-  </si>
-  <si>
-    <t>&lt;i&gt;</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
@@ -47,9 +129,6 @@
     <t>example value</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -83,18 +162,12 @@
     <t xml:space="preserve"> &lt;derived from file&gt;</t>
   </si>
   <si>
-    <t>centre of lowest gate + platform deployment height</t>
-  </si>
-  <si>
     <t>valid_max</t>
   </si>
   <si>
     <t xml:space="preserve"> &lt;derived from file&gt; </t>
   </si>
   <si>
-    <t>centre of highest gate + platform deployment height</t>
-  </si>
-  <si>
     <t>coordinates</t>
   </si>
   <si>
@@ -158,6 +231,30 @@
     <t>Sensor Zenith Angle (from vertical)</t>
   </si>
   <si>
+    <t>sensor_azimuth_angle</t>
+  </si>
+  <si>
+    <t>Sensor Azimuth Angle (clockwise from true North)</t>
+  </si>
+  <si>
+    <t>profile_pulses</t>
+  </si>
+  <si>
+    <t>Number of pulses in each profile</t>
+  </si>
+  <si>
+    <t>time: sum</t>
+  </si>
+  <si>
+    <t>profile_scaling</t>
+  </si>
+  <si>
+    <t>Scaling of range profile (default = 100%)</t>
+  </si>
+  <si>
+    <t>time: point</t>
+  </si>
+  <si>
     <t>window_contamination</t>
   </si>
   <si>
@@ -167,19 +264,31 @@
     <t>Window Contamination (mV as measured by ADC: 0 - 2500)</t>
   </si>
   <si>
+    <t>window_transmittance</t>
+  </si>
+  <si>
+    <t>Window Transmittance, % of nominal value</t>
+  </si>
+  <si>
     <t>background_light</t>
   </si>
   <si>
     <t>Background Light (mV as measured by ADC: 0 - 2500)</t>
   </si>
   <si>
+    <t>backscatter_sum</t>
+  </si>
+  <si>
+    <t>sr-1</t>
+  </si>
+  <si>
+    <t>Sum of detected and normalized backscatter</t>
+  </si>
+  <si>
     <t>qc_flag</t>
   </si>
   <si>
     <t>byte</t>
-  </si>
-  <si>
-    <t>time, index</t>
   </si>
   <si>
     <t>Data Quality flag</t>
@@ -205,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -213,7 +322,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -226,16 +334,38 @@
     </font>
     <font>
       <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -247,11 +377,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -261,7 +409,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -279,10 +427,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -291,10 +436,10 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -309,7 +454,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -337,7 +482,166 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.29"/>
+    <col customWidth="1" min="2" max="2" width="28.71"/>
+    <col customWidth="1" min="3" max="3" width="29.0"/>
+    <col customWidth="1" min="4" max="4" width="29.71"/>
+    <col customWidth="1" min="5" max="5" width="29.14"/>
+    <col customWidth="1" min="6" max="6" width="28.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -354,72 +658,72 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1"/>
@@ -1424,7 +1728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1444,865 +1748,1226 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>42</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="10">
+        <v>44</v>
+      </c>
+      <c r="C8" s="16">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="B10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="B11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="14"/>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>28</v>
+      <c r="A12" s="11"/>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>29</v>
+      <c r="A14" s="21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="16" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" ht="12.0" customHeight="1">
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="18">
+        <v>44</v>
+      </c>
+      <c r="C20" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" ht="12.0" customHeight="1">
       <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" ht="12.0" customHeight="1">
       <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" ht="12.0" customHeight="1">
       <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" ht="12.0" customHeight="1">
-      <c r="C25" s="17"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" ht="12.0" customHeight="1">
-      <c r="A26" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="17"/>
+      <c r="A26" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="22"/>
     </row>
     <row r="27" ht="12.0" customHeight="1">
       <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" ht="12.0" customHeight="1">
       <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" ht="12.0" customHeight="1">
       <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="20">
+        <v>29</v>
+      </c>
+      <c r="C29" s="25">
         <v>1.0</v>
       </c>
     </row>
     <row r="30" ht="12.0" customHeight="1">
       <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="16" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31" ht="12.0" customHeight="1">
       <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="32" ht="12.0" customHeight="1">
       <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="18">
+        <v>44</v>
+      </c>
+      <c r="C32" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="33" ht="12.0" customHeight="1">
       <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" ht="12.0" customHeight="1">
       <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" ht="12.0" customHeight="1">
       <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" ht="12.0" customHeight="1">
       <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" ht="12.0" customHeight="1">
-      <c r="C37" s="17"/>
+      <c r="C37" s="22"/>
     </row>
     <row r="38" ht="12.0" customHeight="1">
       <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="17"/>
+        <v>62</v>
+      </c>
+      <c r="C38" s="22"/>
     </row>
     <row r="39" ht="12.0" customHeight="1">
       <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" ht="12.0" customHeight="1">
       <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" ht="12.0" customHeight="1">
       <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="42" ht="12.0" customHeight="1">
       <c r="B42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="C42" s="22"/>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" ht="12.0" customHeight="1">
       <c r="B43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" ht="12.0" customHeight="1">
       <c r="B44" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" s="18">
+        <v>44</v>
+      </c>
+      <c r="C44" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="45" ht="12.0" customHeight="1">
       <c r="B45" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" ht="12.0" customHeight="1">
       <c r="B46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" ht="12.0" customHeight="1">
       <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="48" ht="12.0" customHeight="1">
       <c r="B48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="49" ht="12.0" customHeight="1"/>
     <row r="50" ht="12.0" customHeight="1">
       <c r="A50" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="C50" s="22"/>
     </row>
     <row r="51" ht="12.0" customHeight="1">
       <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="52" ht="12.0" customHeight="1">
       <c r="B52" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="53" ht="12.0" customHeight="1">
       <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>43</v>
+        <v>29</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="54" ht="12.0" customHeight="1">
       <c r="B54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="C54" s="22"/>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" ht="12.0" customHeight="1">
       <c r="B55" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="56" ht="12.0" customHeight="1">
       <c r="B56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C56" s="18">
+        <v>44</v>
+      </c>
+      <c r="C56" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="57" ht="12.0" customHeight="1">
       <c r="B57" t="s">
-        <v>21</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="58" ht="12.0" customHeight="1">
       <c r="B58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="59" ht="12.0" customHeight="1">
       <c r="B59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="60" ht="12.0" customHeight="1">
       <c r="B60" t="s">
-        <v>27</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="61" ht="12.0" customHeight="1"/>
     <row r="62" ht="12.0" customHeight="1">
-      <c r="A62" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="17"/>
+      <c r="A62" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="22"/>
     </row>
     <row r="63" ht="12.0" customHeight="1">
       <c r="B63" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="64" ht="12.0" customHeight="1">
       <c r="B64" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="65" ht="12.0" customHeight="1">
       <c r="B65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>46</v>
+        <v>29</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="66" ht="12.0" customHeight="1">
       <c r="B66" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="67" ht="12.0" customHeight="1">
       <c r="B67" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="68" ht="12.0" customHeight="1">
       <c r="B68" t="s">
-        <v>18</v>
-      </c>
-      <c r="C68" s="18">
+        <v>44</v>
+      </c>
+      <c r="C68" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="69" ht="12.0" customHeight="1">
       <c r="B69" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="70" ht="12.0" customHeight="1">
       <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" s="21" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="71" ht="12.0" customHeight="1">
       <c r="B71" t="s">
-        <v>34</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="72" ht="12.0" customHeight="1">
       <c r="B72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="73" ht="12.0" customHeight="1"/>
     <row r="74" ht="12.0" customHeight="1">
-      <c r="A74" t="s">
-        <v>48</v>
-      </c>
-      <c r="C74" s="17"/>
+      <c r="A74" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="22"/>
     </row>
     <row r="75" ht="12.0" customHeight="1">
       <c r="B75" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="76" ht="12.0" customHeight="1">
       <c r="B76" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="77" ht="12.0" customHeight="1">
       <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>49</v>
+        <v>29</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="78" ht="12.0" customHeight="1">
       <c r="B78" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" s="17"/>
-      <c r="D78" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="79" ht="12.0" customHeight="1">
       <c r="B79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="80" ht="12.0" customHeight="1">
       <c r="B80" t="s">
-        <v>18</v>
-      </c>
-      <c r="C80" s="18">
+        <v>44</v>
+      </c>
+      <c r="C80" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="81" ht="12.0" customHeight="1">
       <c r="B81" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="82" ht="12.0" customHeight="1">
       <c r="B82" t="s">
-        <v>24</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="83" ht="12.0" customHeight="1">
       <c r="B83" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="84" ht="12.0" customHeight="1">
       <c r="B84" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="85" ht="12.0" customHeight="1"/>
     <row r="86" ht="12.0" customHeight="1">
-      <c r="A86" t="s">
-        <v>51</v>
-      </c>
-      <c r="C86" s="17"/>
+      <c r="A86" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="22"/>
     </row>
     <row r="87" ht="12.0" customHeight="1">
       <c r="B87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="88" ht="12.0" customHeight="1">
       <c r="B88" t="s">
-        <v>14</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="89" ht="12.0" customHeight="1">
       <c r="B89" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>49</v>
+        <v>29</v>
+      </c>
+      <c r="C89" s="25">
+        <v>1.0</v>
       </c>
     </row>
     <row r="90" ht="12.0" customHeight="1">
       <c r="B90" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="17"/>
-      <c r="D90" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" ht="12.0" customHeight="1">
       <c r="B91" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="16" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="92" ht="12.0" customHeight="1">
       <c r="B92" t="s">
-        <v>18</v>
-      </c>
-      <c r="C92" s="18">
+        <v>44</v>
+      </c>
+      <c r="C92" s="23">
         <v>-1.0E20</v>
       </c>
     </row>
     <row r="93" ht="12.0" customHeight="1">
       <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="C93" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="94" ht="12.0" customHeight="1">
       <c r="B94" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="21" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="95" ht="12.0" customHeight="1">
       <c r="B95" t="s">
-        <v>34</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="96" ht="12.0" customHeight="1">
       <c r="B96" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="97" ht="12.0" customHeight="1"/>
     <row r="98" ht="12.0" customHeight="1">
-      <c r="A98" t="s">
-        <v>53</v>
-      </c>
-      <c r="C98" s="17"/>
+      <c r="A98" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C98" s="22"/>
     </row>
     <row r="99" ht="12.0" customHeight="1">
       <c r="B99" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="100" ht="12.0" customHeight="1">
       <c r="B100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C100" s="17" t="s">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="101" ht="12.0" customHeight="1">
       <c r="B101" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101" s="22">
-        <v>1.0</v>
+        <v>29</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="102" ht="12.0" customHeight="1">
       <c r="B102" t="s">
-        <v>15</v>
-      </c>
-      <c r="C102" s="22"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="103" ht="12.0" customHeight="1">
       <c r="B103" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="17" t="s">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="104" ht="12.0" customHeight="1">
-      <c r="B104" s="11" t="s">
+      <c r="B104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C104" s="23">
+        <v>-1.0E20</v>
+      </c>
+    </row>
+    <row r="105" ht="12.0" customHeight="1">
+      <c r="B105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C104" s="15" t="s">
+    </row>
+    <row r="106" ht="12.0" customHeight="1">
+      <c r="B106" t="s">
+        <v>49</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="107" ht="12.0" customHeight="1">
+      <c r="B107" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="105" ht="12.0" customHeight="1">
-      <c r="B105" s="23" t="s">
+      <c r="C107" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="108" ht="12.0" customHeight="1">
+      <c r="B108" t="s">
+        <v>51</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" ht="12.0" customHeight="1"/>
+    <row r="110" ht="12.0" customHeight="1">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" ht="12.0" customHeight="1">
+      <c r="B111" t="s">
+        <v>38</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" ht="12.0" customHeight="1">
+      <c r="B112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C112" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="113" ht="12.0" customHeight="1">
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="114" ht="12.0" customHeight="1">
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114" s="22"/>
+      <c r="D114" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="115" ht="12.0" customHeight="1">
+      <c r="B115" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="116" ht="12.0" customHeight="1">
+      <c r="B116" t="s">
+        <v>44</v>
+      </c>
+      <c r="C116" s="23">
+        <v>-1.0E20</v>
+      </c>
+    </row>
+    <row r="117" ht="12.0" customHeight="1">
+      <c r="B117" t="s">
+        <v>47</v>
+      </c>
+      <c r="C117" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" ht="12.0" customHeight="1">
+      <c r="B118" t="s">
+        <v>49</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" ht="12.0" customHeight="1">
+      <c r="B119" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C105" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="106" ht="12.0" customHeight="1"/>
-    <row r="107" ht="12.0" customHeight="1"/>
-    <row r="108" ht="12.0" customHeight="1"/>
-    <row r="109" ht="12.0" customHeight="1"/>
-    <row r="110" ht="12.0" customHeight="1"/>
-    <row r="111" ht="12.0" customHeight="1"/>
-    <row r="112" ht="12.0" customHeight="1"/>
-    <row r="113" ht="12.0" customHeight="1"/>
-    <row r="114" ht="12.0" customHeight="1"/>
-    <row r="115" ht="12.0" customHeight="1"/>
-    <row r="116" ht="12.0" customHeight="1"/>
-    <row r="117" ht="12.0" customHeight="1"/>
-    <row r="118" ht="12.0" customHeight="1"/>
-    <row r="119" ht="12.0" customHeight="1"/>
-    <row r="120" ht="12.0" customHeight="1"/>
+    </row>
+    <row r="120" ht="12.0" customHeight="1">
+      <c r="B120" t="s">
+        <v>51</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="121" ht="12.0" customHeight="1"/>
-    <row r="122" ht="12.0" customHeight="1"/>
-    <row r="123" ht="12.0" customHeight="1"/>
-    <row r="124" ht="12.0" customHeight="1"/>
-    <row r="125" ht="12.0" customHeight="1"/>
-    <row r="126" ht="12.0" customHeight="1"/>
-    <row r="127" ht="12.0" customHeight="1"/>
-    <row r="128" ht="12.0" customHeight="1"/>
-    <row r="129" ht="12.0" customHeight="1"/>
-    <row r="130" ht="12.0" customHeight="1"/>
-    <row r="131" ht="12.0" customHeight="1"/>
-    <row r="132" ht="12.0" customHeight="1"/>
+    <row r="122" ht="12.0" customHeight="1">
+      <c r="A122" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C122" s="22"/>
+    </row>
+    <row r="123" ht="12.0" customHeight="1">
+      <c r="B123" t="s">
+        <v>38</v>
+      </c>
+      <c r="C123" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="124" ht="12.0" customHeight="1">
+      <c r="B124" t="s">
+        <v>40</v>
+      </c>
+      <c r="C124" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="125" ht="12.0" customHeight="1">
+      <c r="B125" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="126" ht="12.0" customHeight="1">
+      <c r="B126" t="s">
+        <v>41</v>
+      </c>
+      <c r="C126" s="22"/>
+    </row>
+    <row r="127" ht="12.0" customHeight="1">
+      <c r="B127" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="128" ht="12.0" customHeight="1">
+      <c r="B128" t="s">
+        <v>44</v>
+      </c>
+      <c r="C128" s="23">
+        <v>-1.0E20</v>
+      </c>
+    </row>
+    <row r="129" ht="12.0" customHeight="1">
+      <c r="B129" t="s">
+        <v>47</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" ht="12.0" customHeight="1">
+      <c r="B130" t="s">
+        <v>49</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" ht="12.0" customHeight="1">
+      <c r="B131" t="s">
+        <v>58</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" ht="12.0" customHeight="1">
+      <c r="B132" t="s">
+        <v>51</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="133" ht="12.0" customHeight="1"/>
-    <row r="134" ht="12.0" customHeight="1"/>
-    <row r="135" ht="12.0" customHeight="1"/>
-    <row r="136" ht="12.0" customHeight="1"/>
-    <row r="137" ht="12.0" customHeight="1"/>
-    <row r="138" ht="12.0" customHeight="1"/>
-    <row r="139" ht="12.0" customHeight="1"/>
-    <row r="140" ht="12.0" customHeight="1"/>
-    <row r="141" ht="12.0" customHeight="1"/>
-    <row r="142" ht="12.0" customHeight="1"/>
-    <row r="143" ht="12.0" customHeight="1"/>
-    <row r="144" ht="12.0" customHeight="1"/>
+    <row r="134" ht="12.0" customHeight="1">
+      <c r="A134" t="s">
+        <v>85</v>
+      </c>
+      <c r="C134" s="22"/>
+    </row>
+    <row r="135" ht="12.0" customHeight="1">
+      <c r="B135" t="s">
+        <v>38</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" ht="12.0" customHeight="1">
+      <c r="B136" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" ht="12.0" customHeight="1">
+      <c r="B137" t="s">
+        <v>29</v>
+      </c>
+      <c r="C137" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="138" ht="12.0" customHeight="1">
+      <c r="B138" t="s">
+        <v>41</v>
+      </c>
+      <c r="C138" s="22"/>
+      <c r="D138" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="139" ht="12.0" customHeight="1">
+      <c r="B139" t="s">
+        <v>42</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="140" ht="12.0" customHeight="1">
+      <c r="B140" t="s">
+        <v>44</v>
+      </c>
+      <c r="C140" s="23">
+        <v>-1.0E20</v>
+      </c>
+    </row>
+    <row r="141" ht="12.0" customHeight="1">
+      <c r="B141" t="s">
+        <v>47</v>
+      </c>
+      <c r="C141" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="142" ht="12.0" customHeight="1">
+      <c r="B142" t="s">
+        <v>49</v>
+      </c>
+      <c r="C142" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="143" ht="12.0" customHeight="1">
+      <c r="B143" t="s">
+        <v>58</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" ht="12.0" customHeight="1">
+      <c r="B144" t="s">
+        <v>51</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="145" ht="12.0" customHeight="1"/>
-    <row r="146" ht="12.0" customHeight="1"/>
-    <row r="147" ht="12.0" customHeight="1"/>
-    <row r="148" ht="12.0" customHeight="1"/>
-    <row r="149" ht="12.0" customHeight="1"/>
-    <row r="150" ht="12.0" customHeight="1"/>
-    <row r="151" ht="12.0" customHeight="1"/>
-    <row r="152" ht="12.0" customHeight="1"/>
-    <row r="153" ht="12.0" customHeight="1"/>
-    <row r="154" ht="12.0" customHeight="1"/>
-    <row r="155" ht="12.0" customHeight="1"/>
-    <row r="156" ht="12.0" customHeight="1"/>
+    <row r="146" ht="12.0" customHeight="1">
+      <c r="A146" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C146" s="22"/>
+    </row>
+    <row r="147" ht="12.0" customHeight="1">
+      <c r="B147" t="s">
+        <v>38</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="148" ht="12.0" customHeight="1">
+      <c r="B148" t="s">
+        <v>40</v>
+      </c>
+      <c r="C148" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="149" ht="12.0" customHeight="1">
+      <c r="B149" t="s">
+        <v>29</v>
+      </c>
+      <c r="C149" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" ht="12.0" customHeight="1">
+      <c r="B150" t="s">
+        <v>41</v>
+      </c>
+      <c r="C150" s="22"/>
+    </row>
+    <row r="151" ht="12.0" customHeight="1">
+      <c r="B151" t="s">
+        <v>42</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="152" ht="12.0" customHeight="1">
+      <c r="B152" t="s">
+        <v>44</v>
+      </c>
+      <c r="C152" s="23">
+        <v>-1.0E20</v>
+      </c>
+    </row>
+    <row r="153" ht="12.0" customHeight="1">
+      <c r="B153" t="s">
+        <v>47</v>
+      </c>
+      <c r="C153" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="154" ht="12.0" customHeight="1">
+      <c r="B154" t="s">
+        <v>49</v>
+      </c>
+      <c r="C154" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="155" ht="12.0" customHeight="1">
+      <c r="B155" t="s">
+        <v>58</v>
+      </c>
+      <c r="C155" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" ht="12.0" customHeight="1">
+      <c r="B156" t="s">
+        <v>51</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="157" ht="12.0" customHeight="1"/>
-    <row r="158" ht="12.0" customHeight="1"/>
-    <row r="159" ht="12.0" customHeight="1"/>
-    <row r="160" ht="12.0" customHeight="1"/>
-    <row r="161" ht="12.0" customHeight="1"/>
-    <row r="162" ht="12.0" customHeight="1"/>
-    <row r="163" ht="12.0" customHeight="1"/>
-    <row r="164" ht="12.0" customHeight="1"/>
-    <row r="165" ht="12.0" customHeight="1"/>
+    <row r="158" ht="12.0" customHeight="1">
+      <c r="A158" t="s">
+        <v>90</v>
+      </c>
+      <c r="C158" s="22"/>
+    </row>
+    <row r="159" ht="12.0" customHeight="1">
+      <c r="B159" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="160" ht="12.0" customHeight="1">
+      <c r="B160" t="s">
+        <v>40</v>
+      </c>
+      <c r="C160" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="161" ht="12.0" customHeight="1">
+      <c r="B161" t="s">
+        <v>29</v>
+      </c>
+      <c r="C161" s="27">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="162" ht="12.0" customHeight="1">
+      <c r="B162" t="s">
+        <v>41</v>
+      </c>
+      <c r="C162" s="27"/>
+    </row>
+    <row r="163" ht="12.0" customHeight="1">
+      <c r="B163" t="s">
+        <v>42</v>
+      </c>
+      <c r="C163" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="164" ht="12.0" customHeight="1">
+      <c r="B164" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C164" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="165" ht="12.0" customHeight="1">
+      <c r="B165" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C165" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="166" ht="12.0" customHeight="1"/>
     <row r="167" ht="12.0" customHeight="1"/>
     <row r="168" ht="12.0" customHeight="1"/>
@@ -3143,6 +3808,66 @@
     <row r="1003" ht="12.0" customHeight="1"/>
     <row r="1004" ht="12.0" customHeight="1"/>
     <row r="1005" ht="12.0" customHeight="1"/>
+    <row r="1006" ht="12.0" customHeight="1"/>
+    <row r="1007" ht="12.0" customHeight="1"/>
+    <row r="1008" ht="12.0" customHeight="1"/>
+    <row r="1009" ht="12.0" customHeight="1"/>
+    <row r="1010" ht="12.0" customHeight="1"/>
+    <row r="1011" ht="12.0" customHeight="1"/>
+    <row r="1012" ht="12.0" customHeight="1"/>
+    <row r="1013" ht="12.0" customHeight="1"/>
+    <row r="1014" ht="12.0" customHeight="1"/>
+    <row r="1015" ht="12.0" customHeight="1"/>
+    <row r="1016" ht="12.0" customHeight="1"/>
+    <row r="1017" ht="12.0" customHeight="1"/>
+    <row r="1018" ht="12.0" customHeight="1"/>
+    <row r="1019" ht="12.0" customHeight="1"/>
+    <row r="1020" ht="12.0" customHeight="1"/>
+    <row r="1021" ht="12.0" customHeight="1"/>
+    <row r="1022" ht="12.0" customHeight="1"/>
+    <row r="1023" ht="12.0" customHeight="1"/>
+    <row r="1024" ht="12.0" customHeight="1"/>
+    <row r="1025" ht="12.0" customHeight="1"/>
+    <row r="1026" ht="12.0" customHeight="1"/>
+    <row r="1027" ht="12.0" customHeight="1"/>
+    <row r="1028" ht="12.0" customHeight="1"/>
+    <row r="1029" ht="12.0" customHeight="1"/>
+    <row r="1030" ht="12.0" customHeight="1"/>
+    <row r="1031" ht="12.0" customHeight="1"/>
+    <row r="1032" ht="12.0" customHeight="1"/>
+    <row r="1033" ht="12.0" customHeight="1"/>
+    <row r="1034" ht="12.0" customHeight="1"/>
+    <row r="1035" ht="12.0" customHeight="1"/>
+    <row r="1036" ht="12.0" customHeight="1"/>
+    <row r="1037" ht="12.0" customHeight="1"/>
+    <row r="1038" ht="12.0" customHeight="1"/>
+    <row r="1039" ht="12.0" customHeight="1"/>
+    <row r="1040" ht="12.0" customHeight="1"/>
+    <row r="1041" ht="12.0" customHeight="1"/>
+    <row r="1042" ht="12.0" customHeight="1"/>
+    <row r="1043" ht="12.0" customHeight="1"/>
+    <row r="1044" ht="12.0" customHeight="1"/>
+    <row r="1045" ht="12.0" customHeight="1"/>
+    <row r="1046" ht="12.0" customHeight="1"/>
+    <row r="1047" ht="12.0" customHeight="1"/>
+    <row r="1048" ht="12.0" customHeight="1"/>
+    <row r="1049" ht="12.0" customHeight="1"/>
+    <row r="1050" ht="12.0" customHeight="1"/>
+    <row r="1051" ht="12.0" customHeight="1"/>
+    <row r="1052" ht="12.0" customHeight="1"/>
+    <row r="1053" ht="12.0" customHeight="1"/>
+    <row r="1054" ht="12.0" customHeight="1"/>
+    <row r="1055" ht="12.0" customHeight="1"/>
+    <row r="1056" ht="12.0" customHeight="1"/>
+    <row r="1057" ht="12.0" customHeight="1"/>
+    <row r="1058" ht="12.0" customHeight="1"/>
+    <row r="1059" ht="12.0" customHeight="1"/>
+    <row r="1060" ht="12.0" customHeight="1"/>
+    <row r="1061" ht="12.0" customHeight="1"/>
+    <row r="1062" ht="12.0" customHeight="1"/>
+    <row r="1063" ht="12.0" customHeight="1"/>
+    <row r="1064" ht="12.0" customHeight="1"/>
+    <row r="1065" ht="12.0" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>